<commit_message>
USe FPDI and TCPDF to create submisison forms
</commit_message>
<xml_diff>
--- a/public/templates/ept_tb_submission_form.xlsx
+++ b/public/templates/ept_tb_submission_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\projects\SystemOne\ept\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E530F5F-BBF0-4FF5-9C46-A58A8D1FA3A3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83B4297-B899-43D4-993B-EEB2C1D8DB53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Date Tested</t>
   </si>
@@ -234,49 +234,10 @@
     </r>
   </si>
   <si>
-    <t>If you are experiencing challenges testing the panel or submitting results please contact</t>
-  </si>
-  <si>
     <t xml:space="preserve">Submission Due Date: </t>
   </si>
   <si>
-    <t>Performance Evaluation Panel ID:  shipment.shipment_code</t>
-  </si>
-  <si>
-    <t>country[participant.country].country_name</t>
-  </si>
-  <si>
-    <t>shipment.lastdate_response</t>
-  </si>
-  <si>
-    <t>participant.participant_name</t>
-  </si>
-  <si>
-    <t>participant.pt_id</t>
-  </si>
-  <si>
-    <t>participant.username</t>
-  </si>
-  <si>
-    <t>participant.password</t>
-  </si>
-  <si>
-    <t>country[participant.country].pecc_details</t>
-  </si>
-  <si>
-    <t>sample[0].sample_label</t>
-  </si>
-  <si>
-    <t>sample[1].sample_label</t>
-  </si>
-  <si>
-    <t>sample[2].sample_label</t>
-  </si>
-  <si>
-    <t>sample[3].sample_label</t>
-  </si>
-  <si>
-    <t>sample[4].sample_label</t>
+    <t xml:space="preserve">Performance Evaluation Panel ID:  </t>
   </si>
 </sst>
 </file>
@@ -285,7 +246,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -899,7 +860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1170,6 +1131,12 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1307,9 +1274,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6711,8 +6675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X1182"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="Z47" sqref="Z47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -6731,38 +6695,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A1" s="132" t="s">
-        <v>55</v>
+      <c r="A1" s="134" t="s">
+        <v>54</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="133" t="s">
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="134"/>
+      <c r="L1" s="135" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="133"/>
-      <c r="N1" s="133"/>
-      <c r="O1" s="135" t="s">
-        <v>56</v>
+      <c r="M1" s="135"/>
+      <c r="N1" s="135"/>
+      <c r="O1" s="137"/>
+      <c r="P1" s="137"/>
+      <c r="Q1" s="137"/>
+      <c r="R1" s="123" t="s">
+        <v>53</v>
       </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="135"/>
-      <c r="R1" s="121" t="s">
-        <v>54</v>
-      </c>
-      <c r="S1" s="121"/>
-      <c r="T1" s="121"/>
-      <c r="U1" s="95" t="s">
-        <v>57</v>
-      </c>
-      <c r="V1" s="95"/>
+      <c r="S1" s="123"/>
+      <c r="T1" s="123"/>
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
       <c r="W1" s="71"/>
       <c r="X1" s="72"/>
     </row>
@@ -6793,90 +6753,88 @@
       <c r="X2" s="72"/>
     </row>
     <row r="3" spans="1:24" s="1" customFormat="1" ht="26.45" customHeight="1">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="112"/>
-      <c r="M3" s="112"/>
-      <c r="N3" s="112"/>
-      <c r="O3" s="112"/>
-      <c r="P3" s="112"/>
-      <c r="Q3" s="112"/>
-      <c r="R3" s="112"/>
-      <c r="S3" s="112"/>
-      <c r="T3" s="112"/>
-      <c r="U3" s="112"/>
-      <c r="V3" s="112"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="114"/>
+      <c r="K3" s="114"/>
+      <c r="L3" s="114"/>
+      <c r="M3" s="114"/>
+      <c r="N3" s="114"/>
+      <c r="O3" s="114"/>
+      <c r="P3" s="114"/>
+      <c r="Q3" s="114"/>
+      <c r="R3" s="114"/>
+      <c r="S3" s="114"/>
+      <c r="T3" s="114"/>
+      <c r="U3" s="114"/>
+      <c r="V3" s="114"/>
       <c r="W3" s="21"/>
       <c r="X3" s="71"/>
     </row>
     <row r="4" spans="1:24" s="1" customFormat="1" ht="8.4499999999999993" customHeight="1" thickBot="1">
-      <c r="A4" s="112"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="112"/>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
+      <c r="A4" s="114"/>
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" s="114"/>
+      <c r="S4" s="114"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
       <c r="W4" s="23"/>
       <c r="X4" s="71"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="123"/>
-      <c r="C5" s="116" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="117"/>
-      <c r="E5" s="117"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="117"/>
-      <c r="H5" s="117"/>
-      <c r="I5" s="117"/>
-      <c r="J5" s="117"/>
-      <c r="K5" s="117"/>
-      <c r="L5" s="118"/>
+      <c r="B5" s="125"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="119"/>
+      <c r="L5" s="120"/>
       <c r="M5" s="18"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="119" t="s">
+      <c r="O5" s="121" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="119"/>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="119"/>
-      <c r="S5" s="119" t="s">
+      <c r="P5" s="121"/>
+      <c r="Q5" s="121"/>
+      <c r="R5" s="121"/>
+      <c r="S5" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="119"/>
-      <c r="U5" s="119"/>
-      <c r="V5" s="119"/>
+      <c r="T5" s="121"/>
+      <c r="U5" s="121"/>
+      <c r="V5" s="121"/>
       <c r="W5" s="73"/>
       <c r="X5" s="74"/>
     </row>
@@ -6895,34 +6853,32 @@
       <c r="L6" s="19"/>
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
-      <c r="O6" s="101"/>
-      <c r="P6" s="101"/>
-      <c r="Q6" s="101"/>
-      <c r="R6" s="101"/>
-      <c r="S6" s="120"/>
-      <c r="T6" s="120"/>
-      <c r="U6" s="120"/>
-      <c r="V6" s="120"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="103"/>
+      <c r="S6" s="122"/>
+      <c r="T6" s="122"/>
+      <c r="U6" s="122"/>
+      <c r="V6" s="122"/>
       <c r="W6" s="73"/>
       <c r="X6" s="74"/>
     </row>
     <row r="7" spans="1:24" ht="18" customHeight="1" thickBot="1">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="123"/>
-      <c r="C7" s="116" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="117"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="118"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="120"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
@@ -6951,46 +6907,44 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
-      <c r="O8" s="102" t="s">
+      <c r="O8" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="P8" s="102"/>
-      <c r="Q8" s="102"/>
-      <c r="R8" s="102"/>
-      <c r="S8" s="102"/>
-      <c r="T8" s="136"/>
-      <c r="U8" s="136"/>
-      <c r="V8" s="136"/>
+      <c r="P8" s="104"/>
+      <c r="Q8" s="104"/>
+      <c r="R8" s="104"/>
+      <c r="S8" s="104"/>
+      <c r="T8" s="138"/>
+      <c r="U8" s="138"/>
+      <c r="V8" s="138"/>
       <c r="W8" s="70"/>
       <c r="X8" s="21"/>
     </row>
     <row r="9" spans="1:24" ht="18" customHeight="1" thickBot="1">
-      <c r="A9" s="96" t="s">
+      <c r="A9" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="98"/>
-      <c r="C9" s="116" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="117"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="117"/>
-      <c r="H9" s="117"/>
-      <c r="I9" s="117"/>
-      <c r="J9" s="117"/>
-      <c r="K9" s="117"/>
-      <c r="L9" s="118"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="119"/>
+      <c r="E9" s="119"/>
+      <c r="F9" s="119"/>
+      <c r="G9" s="119"/>
+      <c r="H9" s="119"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="119"/>
+      <c r="L9" s="120"/>
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
-      <c r="O9" s="103"/>
-      <c r="P9" s="103"/>
-      <c r="Q9" s="103"/>
-      <c r="R9" s="103"/>
-      <c r="S9" s="103"/>
-      <c r="T9" s="137"/>
-      <c r="U9" s="137"/>
-      <c r="V9" s="137"/>
+      <c r="O9" s="105"/>
+      <c r="P9" s="105"/>
+      <c r="Q9" s="105"/>
+      <c r="R9" s="105"/>
+      <c r="S9" s="105"/>
+      <c r="T9" s="139"/>
+      <c r="U9" s="139"/>
+      <c r="V9" s="139"/>
       <c r="W9" s="70"/>
       <c r="X9" s="8"/>
     </row>
@@ -7009,48 +6963,46 @@
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
-      <c r="O10" s="103" t="s">
+      <c r="O10" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="P10" s="103"/>
-      <c r="Q10" s="103"/>
-      <c r="R10" s="103"/>
-      <c r="S10" s="103"/>
-      <c r="T10" s="138"/>
-      <c r="U10" s="138"/>
-      <c r="V10" s="138"/>
+      <c r="P10" s="105"/>
+      <c r="Q10" s="105"/>
+      <c r="R10" s="105"/>
+      <c r="S10" s="105"/>
+      <c r="T10" s="140"/>
+      <c r="U10" s="140"/>
+      <c r="V10" s="140"/>
       <c r="W10" s="18"/>
       <c r="X10" s="4"/>
     </row>
     <row r="11" spans="1:24" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A11" s="96" t="s">
+      <c r="A11" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="98"/>
-      <c r="C11" s="116" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="117"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="117"/>
-      <c r="G11" s="117"/>
-      <c r="H11" s="117"/>
-      <c r="I11" s="117"/>
-      <c r="J11" s="117"/>
-      <c r="K11" s="117"/>
-      <c r="L11" s="118"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="119"/>
+      <c r="E11" s="119"/>
+      <c r="F11" s="119"/>
+      <c r="G11" s="119"/>
+      <c r="H11" s="119"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="120"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="104" t="s">
+      <c r="O11" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="P11" s="104"/>
-      <c r="Q11" s="104"/>
-      <c r="R11" s="104"/>
-      <c r="S11" s="104"/>
-      <c r="T11" s="139"/>
-      <c r="U11" s="139"/>
-      <c r="V11" s="139"/>
+      <c r="P11" s="106"/>
+      <c r="Q11" s="106"/>
+      <c r="R11" s="106"/>
+      <c r="S11" s="106"/>
+      <c r="T11" s="141"/>
+      <c r="U11" s="141"/>
+      <c r="V11" s="141"/>
       <c r="W11" s="18"/>
       <c r="X11" s="9"/>
     </row>
@@ -7081,36 +7033,36 @@
       <c r="X12" s="8"/>
     </row>
     <row r="13" spans="1:24" ht="31.15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="127"/>
-      <c r="B13" s="128"/>
-      <c r="C13" s="124" t="s">
+      <c r="A13" s="129"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="125"/>
-      <c r="E13" s="125"/>
-      <c r="F13" s="125"/>
-      <c r="G13" s="126"/>
-      <c r="H13" s="110" t="s">
+      <c r="D13" s="127"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
+      <c r="G13" s="128"/>
+      <c r="H13" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="113" t="s">
+      <c r="I13" s="113"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="113"/>
+      <c r="L13" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="M13" s="114"/>
-      <c r="N13" s="114"/>
-      <c r="O13" s="115"/>
-      <c r="P13" s="129" t="s">
+      <c r="M13" s="116"/>
+      <c r="N13" s="116"/>
+      <c r="O13" s="117"/>
+      <c r="P13" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="Q13" s="130"/>
-      <c r="R13" s="130"/>
-      <c r="S13" s="130"/>
-      <c r="T13" s="130"/>
-      <c r="U13" s="130"/>
-      <c r="V13" s="131"/>
+      <c r="Q13" s="132"/>
+      <c r="R13" s="132"/>
+      <c r="S13" s="132"/>
+      <c r="T13" s="132"/>
+      <c r="U13" s="132"/>
+      <c r="V13" s="133"/>
       <c r="W13" s="74"/>
       <c r="X13" s="21"/>
     </row>
@@ -7188,7 +7140,7 @@
       <c r="A15" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="140">
+      <c r="B15" s="94">
         <v>43235</v>
       </c>
       <c r="C15" s="41"/>
@@ -7229,9 +7181,7 @@
       <c r="X15" s="21"/>
     </row>
     <row r="16" spans="1:24" s="1" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A16" s="32" t="s">
-        <v>63</v>
-      </c>
+      <c r="A16" s="32"/>
       <c r="B16" s="24"/>
       <c r="C16" s="44"/>
       <c r="D16" s="45"/>
@@ -7257,9 +7207,7 @@
       <c r="X16" s="8"/>
     </row>
     <row r="17" spans="1:24" s="1" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A17" s="32" t="s">
-        <v>64</v>
-      </c>
+      <c r="A17" s="32"/>
       <c r="B17" s="27"/>
       <c r="C17" s="44"/>
       <c r="D17" s="45"/>
@@ -7285,9 +7233,7 @@
       <c r="X17" s="8"/>
     </row>
     <row r="18" spans="1:24" s="1" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A18" s="32" t="s">
-        <v>65</v>
-      </c>
+      <c r="A18" s="32"/>
       <c r="B18" s="27"/>
       <c r="C18" s="44"/>
       <c r="D18" s="45"/>
@@ -7313,9 +7259,7 @@
       <c r="X18" s="8"/>
     </row>
     <row r="19" spans="1:24" s="1" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A19" s="32" t="s">
-        <v>66</v>
-      </c>
+      <c r="A19" s="32"/>
       <c r="B19" s="27"/>
       <c r="C19" s="44"/>
       <c r="D19" s="45"/>
@@ -7341,9 +7285,7 @@
       <c r="X19" s="8"/>
     </row>
     <row r="20" spans="1:24" s="1" customFormat="1" ht="21.6" customHeight="1" thickBot="1">
-      <c r="A20" s="32" t="s">
-        <v>67</v>
-      </c>
+      <c r="A20" s="95"/>
       <c r="B20" s="28"/>
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
@@ -7395,10 +7337,10 @@
       <c r="X21" s="8"/>
     </row>
     <row r="22" spans="1:24" s="1" customFormat="1">
-      <c r="A22" s="134" t="s">
+      <c r="A22" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="134"/>
+      <c r="B22" s="136"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -7475,26 +7417,26 @@
       <c r="X24" s="8"/>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="108" t="s">
+      <c r="A25" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="108"/>
-      <c r="C25" s="108"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="108"/>
-      <c r="F25" s="108"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="108"/>
-      <c r="I25" s="108"/>
-      <c r="J25" s="108"/>
-      <c r="K25" s="108"/>
-      <c r="L25" s="108"/>
-      <c r="M25" s="108"/>
-      <c r="N25" s="108"/>
-      <c r="O25" s="108"/>
-      <c r="P25" s="108"/>
-      <c r="Q25" s="108"/>
-      <c r="R25" s="108"/>
+      <c r="B25" s="110"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="110"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="110"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="110"/>
+      <c r="I25" s="110"/>
+      <c r="J25" s="110"/>
+      <c r="K25" s="110"/>
+      <c r="L25" s="110"/>
+      <c r="M25" s="110"/>
+      <c r="N25" s="110"/>
+      <c r="O25" s="110"/>
+      <c r="P25" s="110"/>
+      <c r="Q25" s="110"/>
+      <c r="R25" s="110"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
@@ -7503,24 +7445,24 @@
       <c r="X25" s="2"/>
     </row>
     <row r="26" spans="1:24" ht="23.25" customHeight="1">
-      <c r="A26" s="109"/>
-      <c r="B26" s="109"/>
-      <c r="C26" s="109"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="109"/>
-      <c r="F26" s="109"/>
-      <c r="G26" s="109"/>
-      <c r="H26" s="109"/>
-      <c r="I26" s="109"/>
-      <c r="J26" s="109"/>
-      <c r="K26" s="109"/>
-      <c r="L26" s="109"/>
-      <c r="M26" s="109"/>
-      <c r="N26" s="109"/>
-      <c r="O26" s="109"/>
-      <c r="P26" s="109"/>
-      <c r="Q26" s="109"/>
-      <c r="R26" s="109"/>
+      <c r="A26" s="111"/>
+      <c r="B26" s="111"/>
+      <c r="C26" s="111"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
+      <c r="G26" s="111"/>
+      <c r="H26" s="111"/>
+      <c r="I26" s="111"/>
+      <c r="J26" s="111"/>
+      <c r="K26" s="111"/>
+      <c r="L26" s="111"/>
+      <c r="M26" s="111"/>
+      <c r="N26" s="111"/>
+      <c r="O26" s="111"/>
+      <c r="P26" s="111"/>
+      <c r="Q26" s="111"/>
+      <c r="R26" s="111"/>
       <c r="S26" s="6"/>
       <c r="T26" s="6"/>
       <c r="U26" s="6"/>
@@ -7557,8 +7499,8 @@
       <c r="X27" s="5"/>
     </row>
     <row r="28" spans="1:24" ht="15" customHeight="1" thickBot="1">
-      <c r="A28" s="106"/>
-      <c r="B28" s="106"/>
+      <c r="A28" s="108"/>
+      <c r="B28" s="108"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -7583,20 +7525,20 @@
       <c r="X28" s="6"/>
     </row>
     <row r="29" spans="1:24" s="1" customFormat="1" ht="43.5" customHeight="1" thickBot="1">
-      <c r="A29" s="96" t="s">
+      <c r="A29" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="97"/>
-      <c r="C29" s="97"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="105"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="99"/>
-      <c r="J29" s="99"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="100"/>
+      <c r="B29" s="99"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="107"/>
+      <c r="F29" s="101"/>
+      <c r="G29" s="101"/>
+      <c r="H29" s="101"/>
+      <c r="I29" s="101"/>
+      <c r="J29" s="101"/>
+      <c r="K29" s="101"/>
+      <c r="L29" s="102"/>
       <c r="M29" s="18"/>
       <c r="N29" s="18"/>
       <c r="O29" s="85"/>
@@ -7637,20 +7579,20 @@
       <c r="X30" s="74"/>
     </row>
     <row r="31" spans="1:24" s="1" customFormat="1" ht="27" customHeight="1" thickBot="1">
-      <c r="A31" s="96" t="s">
+      <c r="A31" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="97"/>
-      <c r="C31" s="97"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="99"/>
-      <c r="J31" s="99"/>
-      <c r="K31" s="99"/>
-      <c r="L31" s="100"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="101"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="101"/>
+      <c r="I31" s="101"/>
+      <c r="J31" s="101"/>
+      <c r="K31" s="101"/>
+      <c r="L31" s="102"/>
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
       <c r="O31" s="85"/>
@@ -7691,20 +7633,20 @@
       <c r="X32" s="21"/>
     </row>
     <row r="33" spans="1:24" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A33" s="96" t="s">
+      <c r="A33" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="97"/>
-      <c r="C33" s="97"/>
-      <c r="D33" s="98"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="99"/>
-      <c r="G33" s="99"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="99"/>
-      <c r="K33" s="99"/>
-      <c r="L33" s="100"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="100"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="101"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="101"/>
+      <c r="I33" s="101"/>
+      <c r="J33" s="101"/>
+      <c r="K33" s="101"/>
+      <c r="L33" s="102"/>
       <c r="M33" s="18"/>
       <c r="N33" s="18"/>
       <c r="O33" s="85"/>
@@ -7719,8 +7661,8 @@
       <c r="X33" s="9"/>
     </row>
     <row r="34" spans="1:24" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A34" s="106"/>
-      <c r="B34" s="106"/>
+      <c r="A34" s="108"/>
+      <c r="B34" s="108"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -7745,22 +7687,22 @@
       <c r="X34" s="6"/>
     </row>
     <row r="35" spans="1:24" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A35" s="96" t="s">
+      <c r="A35" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="97"/>
-      <c r="C35" s="97"/>
-      <c r="D35" s="98"/>
-      <c r="E35" s="99" t="s">
+      <c r="B35" s="99"/>
+      <c r="C35" s="99"/>
+      <c r="D35" s="100"/>
+      <c r="E35" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="99"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="99"/>
-      <c r="J35" s="99"/>
-      <c r="K35" s="99"/>
-      <c r="L35" s="100"/>
+      <c r="F35" s="101"/>
+      <c r="G35" s="101"/>
+      <c r="H35" s="101"/>
+      <c r="I35" s="101"/>
+      <c r="J35" s="101"/>
+      <c r="K35" s="101"/>
+      <c r="L35" s="102"/>
       <c r="M35" s="18"/>
       <c r="N35" s="18"/>
       <c r="O35" s="86"/>
@@ -7801,22 +7743,22 @@
       <c r="X36" s="4"/>
     </row>
     <row r="37" spans="1:24" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A37" s="96" t="s">
+      <c r="A37" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="97"/>
-      <c r="C37" s="97"/>
-      <c r="D37" s="98"/>
-      <c r="E37" s="99" t="s">
+      <c r="B37" s="99"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="F37" s="99"/>
-      <c r="G37" s="99"/>
-      <c r="H37" s="99"/>
-      <c r="I37" s="99"/>
-      <c r="J37" s="99"/>
-      <c r="K37" s="99"/>
-      <c r="L37" s="100"/>
+      <c r="F37" s="101"/>
+      <c r="G37" s="101"/>
+      <c r="H37" s="101"/>
+      <c r="I37" s="101"/>
+      <c r="J37" s="101"/>
+      <c r="K37" s="101"/>
+      <c r="L37" s="102"/>
       <c r="M37" s="18"/>
       <c r="N37" s="18"/>
       <c r="O37" s="86"/>
@@ -7857,20 +7799,20 @@
       <c r="X38" s="4"/>
     </row>
     <row r="39" spans="1:24" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A39" s="96" t="s">
+      <c r="A39" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="97"/>
-      <c r="C39" s="97"/>
-      <c r="D39" s="98"/>
-      <c r="E39" s="105"/>
-      <c r="F39" s="99"/>
-      <c r="G39" s="99"/>
-      <c r="H39" s="99"/>
-      <c r="I39" s="99"/>
-      <c r="J39" s="99"/>
-      <c r="K39" s="99"/>
-      <c r="L39" s="100"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="99"/>
+      <c r="D39" s="100"/>
+      <c r="E39" s="107"/>
+      <c r="F39" s="101"/>
+      <c r="G39" s="101"/>
+      <c r="H39" s="101"/>
+      <c r="I39" s="101"/>
+      <c r="J39" s="101"/>
+      <c r="K39" s="101"/>
+      <c r="L39" s="102"/>
       <c r="M39" s="18"/>
       <c r="N39" s="18"/>
       <c r="O39" s="85"/>
@@ -7885,8 +7827,8 @@
       <c r="X39" s="9"/>
     </row>
     <row r="40" spans="1:24" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A40" s="106"/>
-      <c r="B40" s="106"/>
+      <c r="A40" s="108"/>
+      <c r="B40" s="108"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -7911,20 +7853,20 @@
       <c r="X40" s="5"/>
     </row>
     <row r="41" spans="1:24" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A41" s="96" t="s">
+      <c r="A41" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="97"/>
-      <c r="C41" s="97"/>
-      <c r="D41" s="98"/>
-      <c r="E41" s="105"/>
-      <c r="F41" s="99"/>
-      <c r="G41" s="99"/>
-      <c r="H41" s="99"/>
-      <c r="I41" s="99"/>
-      <c r="J41" s="99"/>
-      <c r="K41" s="99"/>
-      <c r="L41" s="100"/>
+      <c r="B41" s="99"/>
+      <c r="C41" s="99"/>
+      <c r="D41" s="100"/>
+      <c r="E41" s="107"/>
+      <c r="F41" s="101"/>
+      <c r="G41" s="101"/>
+      <c r="H41" s="101"/>
+      <c r="I41" s="101"/>
+      <c r="J41" s="101"/>
+      <c r="K41" s="101"/>
+      <c r="L41" s="102"/>
       <c r="M41" s="18"/>
       <c r="N41" s="18"/>
       <c r="O41" s="85"/>
@@ -7965,20 +7907,20 @@
       <c r="X42" s="74"/>
     </row>
     <row r="43" spans="1:24" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A43" s="96" t="s">
+      <c r="A43" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="97"/>
-      <c r="C43" s="97"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="105"/>
-      <c r="F43" s="99"/>
-      <c r="G43" s="99"/>
-      <c r="H43" s="99"/>
-      <c r="I43" s="99"/>
-      <c r="J43" s="99"/>
-      <c r="K43" s="99"/>
-      <c r="L43" s="100"/>
+      <c r="B43" s="99"/>
+      <c r="C43" s="99"/>
+      <c r="D43" s="100"/>
+      <c r="E43" s="107"/>
+      <c r="F43" s="101"/>
+      <c r="G43" s="101"/>
+      <c r="H43" s="101"/>
+      <c r="I43" s="101"/>
+      <c r="J43" s="101"/>
+      <c r="K43" s="101"/>
+      <c r="L43" s="102"/>
       <c r="M43" s="18"/>
       <c r="N43" s="18"/>
       <c r="O43" s="85"/>
@@ -8019,22 +7961,22 @@
       <c r="X44" s="21"/>
     </row>
     <row r="45" spans="1:24" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A45" s="96" t="s">
+      <c r="A45" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="97"/>
-      <c r="C45" s="97"/>
-      <c r="D45" s="98"/>
-      <c r="E45" s="99" t="s">
+      <c r="B45" s="99"/>
+      <c r="C45" s="99"/>
+      <c r="D45" s="100"/>
+      <c r="E45" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="F45" s="99"/>
-      <c r="G45" s="99"/>
-      <c r="H45" s="99"/>
-      <c r="I45" s="99"/>
-      <c r="J45" s="99"/>
-      <c r="K45" s="99"/>
-      <c r="L45" s="100"/>
+      <c r="F45" s="101"/>
+      <c r="G45" s="101"/>
+      <c r="H45" s="101"/>
+      <c r="I45" s="101"/>
+      <c r="J45" s="101"/>
+      <c r="K45" s="101"/>
+      <c r="L45" s="102"/>
       <c r="M45" s="18"/>
       <c r="N45" s="18"/>
       <c r="O45" s="85"/>
@@ -8075,20 +8017,20 @@
       <c r="X46" s="21"/>
     </row>
     <row r="47" spans="1:24" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A47" s="96" t="s">
+      <c r="A47" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="97"/>
-      <c r="C47" s="97"/>
-      <c r="D47" s="98"/>
-      <c r="E47" s="99"/>
-      <c r="F47" s="99"/>
-      <c r="G47" s="99"/>
-      <c r="H47" s="99"/>
-      <c r="I47" s="99"/>
-      <c r="J47" s="99"/>
-      <c r="K47" s="99"/>
-      <c r="L47" s="100"/>
+      <c r="B47" s="99"/>
+      <c r="C47" s="99"/>
+      <c r="D47" s="100"/>
+      <c r="E47" s="101"/>
+      <c r="F47" s="101"/>
+      <c r="G47" s="101"/>
+      <c r="H47" s="101"/>
+      <c r="I47" s="101"/>
+      <c r="J47" s="101"/>
+      <c r="K47" s="101"/>
+      <c r="L47" s="102"/>
       <c r="M47" s="18"/>
       <c r="N47" s="18"/>
       <c r="O47" s="85"/>
@@ -8103,8 +8045,8 @@
       <c r="X47" s="9"/>
     </row>
     <row r="48" spans="1:24" s="1" customFormat="1">
-      <c r="A48" s="122"/>
-      <c r="B48" s="122"/>
+      <c r="A48" s="124"/>
+      <c r="B48" s="124"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -8129,9 +8071,7 @@
       <c r="X48" s="6"/>
     </row>
     <row r="49" spans="1:24" s="1" customFormat="1">
-      <c r="A49" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -8146,15 +8086,13 @@
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
-      <c r="P49" s="94" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q49" s="94"/>
-      <c r="R49" s="94"/>
-      <c r="S49" s="94"/>
-      <c r="T49" s="94"/>
-      <c r="U49" s="94"/>
-      <c r="V49" s="94"/>
+      <c r="P49" s="96"/>
+      <c r="Q49" s="96"/>
+      <c r="R49" s="96"/>
+      <c r="S49" s="96"/>
+      <c r="T49" s="96"/>
+      <c r="U49" s="96"/>
+      <c r="V49" s="96"/>
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
     </row>
@@ -8211,8 +8149,8 @@
       <c r="X51" s="80"/>
     </row>
     <row r="52" spans="1:24" s="1" customFormat="1">
-      <c r="A52" s="107"/>
-      <c r="B52" s="107"/>
+      <c r="A52" s="109"/>
+      <c r="B52" s="109"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -37681,7 +37619,7 @@
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"-,Bold"&amp;16Xpert® MTB/RIF Performance Evaluation Result Form</oddHeader>
-    <oddFooter xml:space="preserve">&amp;LILB-500-FXXA v00&amp;R&amp;K000000Effective Date:  </oddFooter>
+    <oddFooter>&amp;LILB/CDC Version 1.0</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -37764,10 +37702,10 @@
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>